<commit_message>
Upgraded to Live Scraping and Universal App ID support
</commit_message>
<xml_diff>
--- a/output/reports/trend_report_20251226.xlsx
+++ b/output/reports/trend_report_20251226.xlsx
@@ -600,94 +600,94 @@
         </is>
       </c>
       <c r="B2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" t="n">
         <v>6</v>
       </c>
-      <c r="C2" t="n">
-        <v>4</v>
-      </c>
       <c r="D2" t="n">
+        <v>7</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
         <v>5</v>
       </c>
-      <c r="E2" t="n">
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2" t="n">
+        <v>4</v>
+      </c>
+      <c r="J2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>4</v>
+      </c>
+      <c r="M2" t="n">
+        <v>2</v>
+      </c>
+      <c r="N2" t="n">
+        <v>6</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>3</v>
+      </c>
+      <c r="R2" t="n">
+        <v>3</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T2" t="n">
+        <v>1</v>
+      </c>
+      <c r="U2" t="n">
+        <v>4</v>
+      </c>
+      <c r="V2" t="n">
+        <v>4</v>
+      </c>
+      <c r="W2" t="n">
+        <v>3</v>
+      </c>
+      <c r="X2" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="n">
         <v>5</v>
       </c>
-      <c r="F2" t="n">
-        <v>3</v>
-      </c>
-      <c r="G2" t="n">
-        <v>7</v>
-      </c>
-      <c r="H2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" t="n">
-        <v>3</v>
-      </c>
-      <c r="J2" t="n">
-        <v>2</v>
-      </c>
-      <c r="K2" t="n">
-        <v>1</v>
-      </c>
-      <c r="L2" t="n">
-        <v>4</v>
-      </c>
-      <c r="M2" t="n">
-        <v>5</v>
-      </c>
-      <c r="N2" t="n">
-        <v>2</v>
-      </c>
-      <c r="O2" t="n">
-        <v>3</v>
-      </c>
-      <c r="P2" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>5</v>
-      </c>
-      <c r="R2" t="n">
-        <v>1</v>
-      </c>
-      <c r="S2" t="n">
-        <v>1</v>
-      </c>
-      <c r="T2" t="n">
-        <v>5</v>
-      </c>
-      <c r="U2" t="n">
-        <v>4</v>
-      </c>
-      <c r="V2" t="n">
-        <v>2</v>
-      </c>
-      <c r="W2" t="n">
-        <v>6</v>
-      </c>
-      <c r="X2" t="n">
-        <v>4</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>2</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>2</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>0</v>
-      </c>
       <c r="AB2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC2" t="n">
         <v>4</v>
       </c>
       <c r="AD2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AF2" t="n">
         <v>4</v>
@@ -700,97 +700,97 @@
         </is>
       </c>
       <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" t="n">
         <v>6</v>
       </c>
-      <c r="C3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" t="n">
-        <v>4</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1</v>
-      </c>
       <c r="F3" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I3" t="n">
+        <v>3</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" t="n">
+        <v>4</v>
+      </c>
+      <c r="L3" t="n">
+        <v>7</v>
+      </c>
+      <c r="M3" t="n">
+        <v>4</v>
+      </c>
+      <c r="N3" t="n">
+        <v>4</v>
+      </c>
+      <c r="O3" t="n">
+        <v>2</v>
+      </c>
+      <c r="P3" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>4</v>
+      </c>
+      <c r="R3" t="n">
         <v>5</v>
       </c>
-      <c r="J3" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" t="n">
-        <v>2</v>
-      </c>
-      <c r="L3" t="n">
-        <v>4</v>
-      </c>
-      <c r="M3" t="n">
-        <v>4</v>
-      </c>
-      <c r="N3" t="n">
-        <v>3</v>
-      </c>
-      <c r="O3" t="n">
-        <v>4</v>
-      </c>
-      <c r="P3" t="n">
+      <c r="S3" t="n">
+        <v>4</v>
+      </c>
+      <c r="T3" t="n">
+        <v>3</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>4</v>
+      </c>
+      <c r="W3" t="n">
+        <v>3</v>
+      </c>
+      <c r="X3" t="n">
         <v>5</v>
       </c>
-      <c r="Q3" t="n">
-        <v>1</v>
-      </c>
-      <c r="R3" t="n">
-        <v>2</v>
-      </c>
-      <c r="S3" t="n">
-        <v>4</v>
-      </c>
-      <c r="T3" t="n">
-        <v>4</v>
-      </c>
-      <c r="U3" t="n">
-        <v>7</v>
-      </c>
-      <c r="V3" t="n">
-        <v>1</v>
-      </c>
-      <c r="W3" t="n">
+      <c r="Y3" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z3" t="n">
         <v>5</v>
       </c>
-      <c r="X3" t="n">
-        <v>4</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>3</v>
-      </c>
-      <c r="Z3" t="n">
-        <v>3</v>
-      </c>
       <c r="AA3" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AB3" t="n">
         <v>2</v>
       </c>
       <c r="AC3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AD3" t="n">
         <v>3</v>
       </c>
       <c r="AE3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AF3" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -800,67 +800,67 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" t="n">
+        <v>4</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>3</v>
+      </c>
+      <c r="I4" t="n">
+        <v>3</v>
+      </c>
+      <c r="J4" t="n">
+        <v>4</v>
+      </c>
+      <c r="K4" t="n">
+        <v>4</v>
+      </c>
+      <c r="L4" t="n">
+        <v>3</v>
+      </c>
+      <c r="M4" t="n">
+        <v>10</v>
+      </c>
+      <c r="N4" t="n">
+        <v>2</v>
+      </c>
+      <c r="O4" t="n">
+        <v>4</v>
+      </c>
+      <c r="P4" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q4" t="n">
         <v>5</v>
       </c>
-      <c r="F4" t="n">
-        <v>2</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" t="n">
-        <v>2</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" t="n">
+      <c r="R4" t="n">
+        <v>6</v>
+      </c>
+      <c r="S4" t="n">
+        <v>4</v>
+      </c>
+      <c r="T4" t="n">
         <v>5</v>
       </c>
-      <c r="K4" t="n">
-        <v>2</v>
-      </c>
-      <c r="L4" t="n">
-        <v>7</v>
-      </c>
-      <c r="M4" t="n">
-        <v>5</v>
-      </c>
-      <c r="N4" t="n">
-        <v>3</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>3</v>
-      </c>
-      <c r="R4" t="n">
-        <v>1</v>
-      </c>
-      <c r="S4" t="n">
-        <v>5</v>
-      </c>
-      <c r="T4" t="n">
-        <v>2</v>
-      </c>
       <c r="U4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="V4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W4" t="n">
         <v>1</v>
@@ -869,28 +869,28 @@
         <v>4</v>
       </c>
       <c r="Y4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Z4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AA4" t="n">
         <v>1</v>
       </c>
       <c r="AB4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AD4" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AE4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AF4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -900,97 +900,97 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E5" t="n">
         <v>2</v>
       </c>
       <c r="F5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" t="n">
         <v>8</v>
       </c>
-      <c r="G5" t="n">
-        <v>4</v>
-      </c>
       <c r="H5" t="n">
         <v>1</v>
       </c>
       <c r="I5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L5" t="n">
+        <v>4</v>
+      </c>
+      <c r="M5" t="n">
+        <v>2</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>2</v>
+      </c>
+      <c r="P5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="n">
         <v>6</v>
       </c>
-      <c r="M5" t="n">
-        <v>2</v>
-      </c>
-      <c r="N5" t="n">
-        <v>1</v>
-      </c>
-      <c r="O5" t="n">
-        <v>2</v>
-      </c>
-      <c r="P5" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>1</v>
-      </c>
       <c r="R5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="T5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V5" t="n">
         <v>2</v>
       </c>
       <c r="W5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="X5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Y5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Z5" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="AA5" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB5" t="n">
         <v>7</v>
       </c>
-      <c r="AB5" t="n">
-        <v>2</v>
-      </c>
       <c r="AC5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD5" t="n">
         <v>2</v>
       </c>
       <c r="AE5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AF5" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -1000,13 +1000,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" t="n">
         <v>4</v>
@@ -1015,82 +1015,82 @@
         <v>2</v>
       </c>
       <c r="G6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H6" t="n">
         <v>1</v>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N6" t="n">
+        <v>2</v>
+      </c>
+      <c r="O6" t="n">
+        <v>1</v>
+      </c>
+      <c r="P6" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>6</v>
+      </c>
+      <c r="R6" t="n">
+        <v>1</v>
+      </c>
+      <c r="S6" t="n">
+        <v>2</v>
+      </c>
+      <c r="T6" t="n">
         <v>0</v>
       </c>
-      <c r="O6" t="n">
-        <v>1</v>
-      </c>
-      <c r="P6" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>3</v>
-      </c>
-      <c r="R6" t="n">
+      <c r="U6" t="n">
+        <v>1</v>
+      </c>
+      <c r="V6" t="n">
+        <v>2</v>
+      </c>
+      <c r="W6" t="n">
+        <v>3</v>
+      </c>
+      <c r="X6" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC6" t="n">
         <v>0</v>
       </c>
-      <c r="S6" t="n">
-        <v>4</v>
-      </c>
-      <c r="T6" t="n">
-        <v>2</v>
-      </c>
-      <c r="U6" t="n">
-        <v>1</v>
-      </c>
-      <c r="V6" t="n">
-        <v>6</v>
-      </c>
-      <c r="W6" t="n">
+      <c r="AD6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF6" t="n">
         <v>0</v>
-      </c>
-      <c r="X6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z6" t="n">
-        <v>3</v>
-      </c>
-      <c r="AA6" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB6" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>2</v>
-      </c>
-      <c r="AE6" t="n">
-        <v>3</v>
-      </c>
-      <c r="AF6" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -1100,97 +1100,97 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" t="n">
         <v>2</v>
       </c>
       <c r="E7" t="n">
+        <v>6</v>
+      </c>
+      <c r="F7" t="n">
+        <v>4</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" t="n">
+        <v>2</v>
+      </c>
+      <c r="J7" t="n">
         <v>5</v>
       </c>
-      <c r="F7" t="n">
-        <v>4</v>
-      </c>
-      <c r="G7" t="n">
-        <v>2</v>
-      </c>
-      <c r="H7" t="n">
-        <v>3</v>
-      </c>
-      <c r="I7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" t="n">
-        <v>4</v>
-      </c>
       <c r="K7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L7" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N7" t="n">
         <v>2</v>
       </c>
       <c r="O7" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q7" t="n">
+        <v>1</v>
+      </c>
+      <c r="R7" t="n">
+        <v>1</v>
+      </c>
+      <c r="S7" t="n">
+        <v>4</v>
+      </c>
+      <c r="T7" t="n">
+        <v>6</v>
+      </c>
+      <c r="U7" t="n">
+        <v>3</v>
+      </c>
+      <c r="V7" t="n">
+        <v>3</v>
+      </c>
+      <c r="W7" t="n">
+        <v>2</v>
+      </c>
+      <c r="X7" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>7</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD7" t="n">
         <v>5</v>
       </c>
-      <c r="R7" t="n">
-        <v>2</v>
-      </c>
-      <c r="S7" t="n">
-        <v>1</v>
-      </c>
-      <c r="T7" t="n">
-        <v>3</v>
-      </c>
-      <c r="U7" t="n">
-        <v>2</v>
-      </c>
-      <c r="V7" t="n">
-        <v>2</v>
-      </c>
-      <c r="W7" t="n">
-        <v>3</v>
-      </c>
-      <c r="X7" t="n">
-        <v>3</v>
-      </c>
-      <c r="Y7" t="n">
-        <v>3</v>
-      </c>
-      <c r="Z7" t="n">
-        <v>2</v>
-      </c>
-      <c r="AA7" t="n">
+      <c r="AE7" t="n">
         <v>5</v>
       </c>
-      <c r="AB7" t="n">
-        <v>6</v>
-      </c>
-      <c r="AC7" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD7" t="n">
-        <v>2</v>
-      </c>
-      <c r="AE7" t="n">
-        <v>2</v>
-      </c>
       <c r="AF7" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -1200,97 +1200,97 @@
         </is>
       </c>
       <c r="B8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>4</v>
+      </c>
+      <c r="E8" t="n">
+        <v>6</v>
+      </c>
+      <c r="F8" t="n">
+        <v>4</v>
+      </c>
+      <c r="G8" t="n">
+        <v>4</v>
+      </c>
+      <c r="H8" t="n">
+        <v>3</v>
+      </c>
+      <c r="I8" t="n">
+        <v>3</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" t="n">
+        <v>3</v>
+      </c>
+      <c r="M8" t="n">
+        <v>3</v>
+      </c>
+      <c r="N8" t="n">
+        <v>3</v>
+      </c>
+      <c r="O8" t="n">
+        <v>2</v>
+      </c>
+      <c r="P8" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>2</v>
+      </c>
+      <c r="R8" t="n">
         <v>0</v>
       </c>
-      <c r="C8" t="n">
-        <v>3</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" t="n">
-        <v>2</v>
-      </c>
-      <c r="F8" t="n">
-        <v>6</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" t="n">
-        <v>2</v>
-      </c>
-      <c r="I8" t="n">
-        <v>3</v>
-      </c>
-      <c r="J8" t="n">
-        <v>3</v>
-      </c>
-      <c r="K8" t="n">
-        <v>5</v>
-      </c>
-      <c r="L8" t="n">
-        <v>2</v>
-      </c>
-      <c r="M8" t="n">
-        <v>1</v>
-      </c>
-      <c r="N8" t="n">
-        <v>4</v>
-      </c>
-      <c r="O8" t="n">
-        <v>5</v>
-      </c>
-      <c r="P8" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>3</v>
-      </c>
-      <c r="R8" t="n">
-        <v>1</v>
-      </c>
       <c r="S8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T8" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="U8" t="n">
         <v>2</v>
       </c>
       <c r="V8" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="W8" t="n">
         <v>3</v>
       </c>
       <c r="X8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Y8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AA8" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AB8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AC8" t="n">
         <v>5</v>
       </c>
       <c r="AD8" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AE8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AF8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1341,7 +1341,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>621</v>
+        <v>636</v>
       </c>
     </row>
     <row r="4">
@@ -1351,7 +1351,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>88.70999999999999</v>
+        <v>90.86</v>
       </c>
     </row>
     <row r="5">
@@ -1362,7 +1362,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Customer support unresponsive</t>
+          <t>Delivery issue</t>
         </is>
       </c>
     </row>
@@ -1385,7 +1385,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -1452,45 +1452,45 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Delivery partner rude</t>
+          <t>Wrong order delivered</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3.29</v>
+        <v>3.71</v>
       </c>
       <c r="C2" t="n">
-        <v>2.57</v>
+        <v>2.14</v>
       </c>
       <c r="D2" t="n">
-        <v>0.28</v>
+        <v>0.73</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>27.8%</t>
+          <t>73.3%</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Payment issue</t>
+          <t>Delivery partner rude</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>2.43</v>
+        <v>3</v>
       </c>
       <c r="D3" t="n">
-        <v>0.24</v>
+        <v>0.33</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>23.5%</t>
+          <t>33.3%</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -1500,73 +1500,73 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Wrong order delivered</t>
+          <t>Payment issue</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3.43</v>
+        <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>2.86</v>
+        <v>3.29</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>20.0%</t>
+          <t>21.7%</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Delivery issue</t>
+          <t>Customer support unresponsive</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2.86</v>
+        <v>3.29</v>
       </c>
       <c r="C5" t="n">
-        <v>2.86</v>
+        <v>3</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>9.5%</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>88</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Food stale</t>
+          <t>Delivery issue</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.71</v>
+        <v>3.43</v>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>3.14</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.14</v>
+        <v>0.09</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>-14.3%</t>
+          <t>9.1%</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>65</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7">
@@ -1576,45 +1576,45 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2.43</v>
+        <v>2.71</v>
       </c>
       <c r="C7" t="n">
-        <v>3.43</v>
+        <v>2.86</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.29</v>
+        <v>-0.05</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>-29.2%</t>
+          <t>-5.0%</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Customer support unresponsive</t>
+          <t>Food stale</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2.57</v>
+        <v>1.29</v>
       </c>
       <c r="C8" t="n">
-        <v>4</v>
+        <v>1.57</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.36</v>
+        <v>-0.18</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>-35.7%</t>
+          <t>-18.2%</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>104</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1656,72 +1656,72 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Customer support unresponsive</t>
+          <t>Delivery issue</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="C2" t="n">
-        <v>3.35</v>
+        <v>3.61</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>App crashing</t>
+          <t>Customer support unresponsive</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C3" t="n">
-        <v>3.26</v>
+        <v>3.45</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Delivery issue</t>
+          <t>App crashing</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C4" t="n">
-        <v>2.84</v>
+        <v>3.06</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Delivery partner rude</t>
+          <t>Payment issue</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C5" t="n">
-        <v>2.84</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Wrong order delivered</t>
+          <t>Delivery partner rude</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C6" t="n">
-        <v>2.84</v>
+        <v>2.81</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Payment issue</t>
+          <t>Wrong order delivered</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1738,10 +1738,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C8" t="n">
-        <v>2.1</v>
+        <v>1.77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>